<commit_message>
Acoustics Work | Library Additions
Added Robot Connector
Created 3rd Page for power
Voltage converters (15 to -15, 15 to 5, 5 to 3.3)
Mixer
Diode to Envelope Detector

Added to Libraries
Capacitors
Diodes
Inductors
Integrated Circuits

Worked on Acoustics BOM
</commit_message>
<xml_diff>
--- a/TempestBoards/Acoustics/Acoustics BOM.xlsx
+++ b/TempestBoards/Acoustics/Acoustics BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\becca\Documents\GitHub\electric_boogaloo\TempestBoards\Acoustics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\Documents\Everything\UWRT\Electrical\GIT\electric_boogaloo\TempestBoards\Acoustics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C28EC0A6-66A4-4DF1-9199-9A8427FA8601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7059A73-E74A-4A79-AEA3-E189E617FE6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12150" yWindow="0" windowWidth="12150" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="175">
   <si>
     <t>Distributor</t>
   </si>
@@ -246,6 +246,339 @@
   </si>
   <si>
     <t>1276-1085-1-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/C0402C101K3GAC7867/399-C0402C101K3GAC7867CT-ND/3471471?curr=usd&amp;utm_campaign=buynow&amp;utm_medium=aggregator&amp;utm_source=octopart</t>
+  </si>
+  <si>
+    <t>399-C0402C101K3GAC7867TR-ND</t>
+  </si>
+  <si>
+    <t>C0402C101K3GAC7867</t>
+  </si>
+  <si>
+    <t>100p Farad Capacitor 0402</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/johanson-technology-inc/LRC0402CJ15NGV001T/1840068</t>
+  </si>
+  <si>
+    <t>15n Henry Inductor 0402</t>
+  </si>
+  <si>
+    <t>712-LRC0402CJ15NGV001TTR-ND</t>
+  </si>
+  <si>
+    <t>LRC0402CJ15NGV001T</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/murata-electronics/LQG15HSR27J02D/662889</t>
+  </si>
+  <si>
+    <t>270n Henry Inductor 0402</t>
+  </si>
+  <si>
+    <t>490-2640-2-ND</t>
+  </si>
+  <si>
+    <t>LQG15HSR27J02D</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/C0603C102K5RAC7867/399-C0603C102K5RAC7867CT-ND/411357?curr=usd&amp;utm_campaign=buynow&amp;utm_medium=aggregator&amp;utm_source=octopart</t>
+  </si>
+  <si>
+    <t>1n Farad Capacitor 0603</t>
+  </si>
+  <si>
+    <t>399-C0603C102K5RAC7867TR-ND</t>
+  </si>
+  <si>
+    <t>C0603C102K5RAC7867</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/johanson-technology-inc/QSCF500Q4R7B1GV001T/1786615</t>
+  </si>
+  <si>
+    <t>4.7p Farad Capacitor 0402</t>
+  </si>
+  <si>
+    <t>712-QSCF500Q4R7B1GV001TTR-ND</t>
+  </si>
+  <si>
+    <t>QSCF500Q4R7B1GV001T</t>
+  </si>
+  <si>
+    <t>1u Farad Capacitor 0603</t>
+  </si>
+  <si>
+    <t>CC0603KRX7R8BB105</t>
+  </si>
+  <si>
+    <t>311-1802-1-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/johanson-technology-inc/LRC0402CJ6N8GV001T/1840077</t>
+  </si>
+  <si>
+    <t>6.8 Henry Capacitor 0402</t>
+  </si>
+  <si>
+    <t>712-LRC0402CJ6N8GV001TTR-ND</t>
+  </si>
+  <si>
+    <t>LRC0402CJ6N8GV001T</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/johanson-technology-inc/QSCP251Q330J1GV001T/1561621</t>
+  </si>
+  <si>
+    <t>33p Farad Capacitor 0603</t>
+  </si>
+  <si>
+    <t>712-QSCP251Q330J1GV001TTR-ND</t>
+  </si>
+  <si>
+    <t>QSCP251Q330J1GV001T</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/analog-devices-inc/LT5560EDD-PBF/1620364</t>
+  </si>
+  <si>
+    <t>RF Mixer</t>
+  </si>
+  <si>
+    <t>505-LT5560EDD#PBF-ND</t>
+  </si>
+  <si>
+    <t>LT5560EDD#PBF</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stackpole-electronics-inc/CSR1206FK12L0/1788085?s=N4IgTCBcDaIMIGUBKBGMAGAbAMQNJoBl0QBdAXyA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/yageo/RC0603FR-078K87L/727394?s=N4IgTCBcDaIEoGEAMA2JBmAYnAtEg7ABwDSh%2BAMiALoC%2BQA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/vishay-dale/CRCW0603787RFKEA/1174656</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL10C561JB8NFNC/3887973?s=N4IgTCBcDaIMIBkCMAGOBWAbEgUgIQA4A5AMSLhAF0BfIA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/panasonic-electronic-components/EEH-ZC1E331P/3088060?s=N4IgTCBcDaIKJwBIC0DCBGOBmL6AKIAugL5A</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/yageo/RC0603FR-071K21L/726854?s=N4IgTCBcDaIEoGEAMA2JBmAYnAtEg7AIwDSYhAMiALoC%2BQA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/vishay-dale/CRCW060313K7FKEA/1174796</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL10C200JB8NNNC/3886845?s=N4IgTCBcDaIMIBkCMAGOYUoFICEAcAckXCALoC%2BQA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL10C221JB8NNNC/3886706?s=N4IgTCBcDaIMIBkCMAGOYxIFICEAcAckXCALoC%2BQA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/yageo/RC0402FR-075K23L/5281055</t>
+  </si>
+  <si>
+    <t>CSR1206FK12L0TR-ND</t>
+  </si>
+  <si>
+    <t>CSR1206FK12L0</t>
+  </si>
+  <si>
+    <t>0.012 Ohm Resistor 1206</t>
+  </si>
+  <si>
+    <t>311-8.87KHRTR-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-078K87L</t>
+  </si>
+  <si>
+    <t>8.87k Ohm Resistor 0603</t>
+  </si>
+  <si>
+    <t>541-787HTR-ND</t>
+  </si>
+  <si>
+    <t>CRCW0603787RFKEA</t>
+  </si>
+  <si>
+    <t>787 Ohm Resistor 0603</t>
+  </si>
+  <si>
+    <t>1276-2315-2-ND</t>
+  </si>
+  <si>
+    <t>CL10C561JB8NFNC</t>
+  </si>
+  <si>
+    <t>P15459TR-ND</t>
+  </si>
+  <si>
+    <t>EEH-ZC1E331P</t>
+  </si>
+  <si>
+    <t>560p Farad Capacitor 0603</t>
+  </si>
+  <si>
+    <t>311-1.21KHRTR-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-071K21L</t>
+  </si>
+  <si>
+    <t>1.21k Ohm Resistor 0603</t>
+  </si>
+  <si>
+    <t>541-13.7KHTR-ND</t>
+  </si>
+  <si>
+    <t>CRCW060313K7FKEA</t>
+  </si>
+  <si>
+    <t>13.7k Ohm Resistor 0603</t>
+  </si>
+  <si>
+    <t>1276-1187-2-ND</t>
+  </si>
+  <si>
+    <t>CL10C200JB8NNNC</t>
+  </si>
+  <si>
+    <t>20p Farad Capacitor 0603</t>
+  </si>
+  <si>
+    <t>1276-1048-2-ND</t>
+  </si>
+  <si>
+    <t>CL10C221JB8NNNC</t>
+  </si>
+  <si>
+    <t>220p Farad Capacitor 0603</t>
+  </si>
+  <si>
+    <t>YAG3195TR-ND</t>
+  </si>
+  <si>
+    <t>RC0402FR-075K23L</t>
+  </si>
+  <si>
+    <t>5.23k Ohm Resistor 0402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">205k Ohm Resistor </t>
+  </si>
+  <si>
+    <t>YAG3050TR-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/yageo/RC0402FR-07205KL/5280910</t>
+  </si>
+  <si>
+    <t>RC0402FR-07205KL</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/texas-instruments/LM1117IMPX-3-3-NOPB/1870906?s=N4IgTCBcDaIDIFkCMKDsBJBAFAGgWgGYA6AgegDkB5LAIRAF0BfIA</t>
+  </si>
+  <si>
+    <t>LM1117IMPX-3.3/NOPBTR-ND</t>
+  </si>
+  <si>
+    <t>LM1117IMPX-3.3/NOPB</t>
+  </si>
+  <si>
+    <t>3.3V Linear Regulator</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL10A225KP8NNNC/3886743?s=N4IgTCBcDaIIxgOwDYC0cAMAOArO1AcgCIgC6AvkA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/yageo/AC0402FR-131KL/14008372?s=N4IgTCBcDaIIwGYC0BBAwgBgCwbAMQCUlE4BpAGTQBUkA5AERAF0BfIA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stackpole-electronics-inc/RNCP0603FTD10K0/2240139?s=N4IgTCBcDaIEoDkDCAFADANjQZgGIBUARARjQGk0l8BaBQkAXQF8g</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/bourns-inc/TC33X-2-103E/612858?s=N4IgTCBcDaICoGEDMSAaBaAjABiQUQTnQDkAREAXQF8g</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/bourns-inc/TC33X-2-203E/2566887?s=N4IgTCBcDaICoGEDMSAaBaMmAMSCiCc6AcgCIgC6AvkA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/murata-electronics/GRM188R60J106ME47J/2612410?s=N4IgTCBcDaICwE4AMBaAbHJBWFBGFAcgCIgC6AvkA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/yageo/CC0603KRX7R8BB105/5195210?s=N4IgTCBcDaIMwEYEFoEA4AMZXIHIBEQBdAXyA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/diodes-incorporated/AZ1117IH-5-0TRG1/5699673</t>
+  </si>
+  <si>
+    <t>AZ1117IH-5.0TRG1DITR-ND</t>
+  </si>
+  <si>
+    <t>AZ1117IH-5.0TRG1</t>
+  </si>
+  <si>
+    <t>5V Fixed LDO</t>
+  </si>
+  <si>
+    <t>PCE3952DKR-ND</t>
+  </si>
+  <si>
+    <t>EEE-1VA220SP</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/panasonic-electronic-components/EEE-1VA220SP/761837?s=N4IgTCBcDaIAoGECiBmAnAVjAEQNICUBaAOWxAF0BfIA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/EEH-ZC1J100P/P15466CT-ND/3088097?curr=usd&amp;utm_campaign=buynow&amp;utm_medium=aggregator&amp;utm_source=octopart</t>
+  </si>
+  <si>
+    <t>P15466TR-ND</t>
+  </si>
+  <si>
+    <t>EEH-ZC1J100P</t>
+  </si>
+  <si>
+    <t>10u Farad Alum Cap</t>
+  </si>
+  <si>
+    <t>22u Farad Alum Cap</t>
+  </si>
+  <si>
+    <t>330u Farad Alum Cap</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/texas-instruments/LM25116MHX-NOPB/1870976</t>
+  </si>
+  <si>
+    <t>296-35258-2-ND</t>
+  </si>
+  <si>
+    <t>LM25116MHX/NOPB</t>
+  </si>
+  <si>
+    <t>DC-DC Buck Regulator</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/infineon-technologies/BAR9002ELE6327XTMA1/4765722</t>
+  </si>
+  <si>
+    <t>Diode</t>
+  </si>
+  <si>
+    <t>BAR9002ELE6327XTMA1TR-ND</t>
+  </si>
+  <si>
+    <t>BAR9002ELE6327XTMA1</t>
+  </si>
+  <si>
+    <t>RF Diode</t>
   </si>
 </sst>
 </file>
@@ -276,10 +609,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="7"/>
+      <sz val="11"/>
       <color rgb="FF222222"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -397,7 +731,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -443,8 +777,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -740,29 +1077,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:M50"/>
+  <dimension ref="B1:M73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.86328125" style="3"/>
-    <col min="2" max="2" width="8.86328125" style="4"/>
-    <col min="3" max="3" width="9.86328125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="15.19921875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="3"/>
+    <col min="2" max="2" width="8.85546875" style="4"/>
+    <col min="3" max="3" width="9.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="4" customWidth="1"/>
     <col min="5" max="5" width="12" style="4" customWidth="1"/>
     <col min="6" max="6" width="18" style="4" customWidth="1"/>
-    <col min="7" max="7" width="23.33203125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
     <col min="9" max="9" width="12" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.86328125" style="7" customWidth="1"/>
-    <col min="11" max="16384" width="8.86328125" style="3"/>
+    <col min="10" max="10" width="9.85546875" style="7" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
@@ -791,7 +1128,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="2:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="2:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="5" t="s">
+        <v>147</v>
+      </c>
       <c r="C2" s="4" t="s">
         <v>11</v>
       </c>
@@ -818,7 +1158,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>16</v>
       </c>
@@ -844,7 +1184,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="7">
-        <f t="shared" ref="J3:J38" si="0">I3-H3</f>
+        <f t="shared" ref="J3:J66" si="0">I3-H3</f>
         <v>-2</v>
       </c>
       <c r="L3" s="11" t="s">
@@ -852,7 +1192,10 @@
       </c>
       <c r="M3" s="12"/>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
+        <v>148</v>
+      </c>
       <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
@@ -883,7 +1226,10 @@
       </c>
       <c r="M4" s="14"/>
     </row>
-    <row r="5" spans="2:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="5" t="s">
+        <v>149</v>
+      </c>
       <c r="C5" s="4" t="s">
         <v>11</v>
       </c>
@@ -914,7 +1260,10 @@
       </c>
       <c r="M5" s="16"/>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
+        <v>150</v>
+      </c>
       <c r="C6" s="4" t="s">
         <v>11</v>
       </c>
@@ -941,18 +1290,37 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>170</v>
+      </c>
       <c r="C7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D7"/>
-      <c r="F7"/>
+      <c r="D7" t="s">
+        <v>172</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="F7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="H7" s="1">
+        <v>2</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
       <c r="J7" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.45">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>30</v>
       </c>
@@ -982,7 +1350,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>37</v>
       </c>
@@ -1012,7 +1380,10 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>151</v>
+      </c>
       <c r="C10" s="4" t="s">
         <v>11</v>
       </c>
@@ -1029,17 +1400,17 @@
         <v>39</v>
       </c>
       <c r="H10" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I10" s="1">
         <v>19</v>
       </c>
       <c r="J10" s="7">
         <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.45">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C11" s="4" t="s">
         <v>11</v>
       </c>
@@ -1048,7 +1419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>51</v>
       </c>
@@ -1078,7 +1449,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>50</v>
       </c>
@@ -1108,7 +1479,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>46</v>
       </c>
@@ -1138,8 +1509,8 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B15" s="17" t="s">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="18" t="s">
         <v>55</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -1151,7 +1522,7 @@
       <c r="E15" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F15" s="18" t="s">
+      <c r="F15" s="17" t="s">
         <v>56</v>
       </c>
       <c r="G15" s="4" t="s">
@@ -1169,7 +1540,7 @@
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="5" t="s">
         <v>58</v>
       </c>
       <c r="C16" s="4" t="s">
@@ -1181,7 +1552,7 @@
       <c r="E16" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="18" t="s">
+      <c r="F16" s="17" t="s">
         <v>60</v>
       </c>
       <c r="G16" s="4" t="s">
@@ -1198,7 +1569,10 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="17" spans="3:10" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="5" t="s">
+        <v>146</v>
+      </c>
       <c r="C17" s="4" t="s">
         <v>11</v>
       </c>
@@ -1208,7 +1582,7 @@
       <c r="E17" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F17" s="10">
+      <c r="F17" s="19">
         <v>58727859</v>
       </c>
       <c r="G17" s="4" t="s">
@@ -1225,7 +1599,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="3:10" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C18" s="4" t="s">
         <v>11</v>
       </c>
@@ -1234,244 +1608,955 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="3:10" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="5" t="s">
+        <v>64</v>
+      </c>
       <c r="C19" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="D19" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H19" s="1">
+        <v>6</v>
+      </c>
+      <c r="I19" s="1">
+        <v>0</v>
+      </c>
       <c r="J19" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="3:10" x14ac:dyDescent="0.45">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="5" t="s">
+        <v>68</v>
+      </c>
       <c r="C20" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="D20" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H20" s="1">
+        <v>4</v>
+      </c>
+      <c r="I20" s="1">
+        <v>0</v>
+      </c>
       <c r="J20" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="3:10" x14ac:dyDescent="0.45">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B21" s="5" t="s">
+        <v>72</v>
+      </c>
       <c r="C21" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="D21" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H21" s="1">
+        <v>6</v>
+      </c>
+      <c r="I21" s="1">
+        <v>0</v>
+      </c>
       <c r="J21" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="3:10" x14ac:dyDescent="0.45">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B22" s="5" t="s">
+        <v>76</v>
+      </c>
       <c r="C22" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="D22" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H22" s="1">
+        <v>2</v>
+      </c>
+      <c r="I22" s="1">
+        <v>0</v>
+      </c>
       <c r="J22" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="3:10" x14ac:dyDescent="0.45">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B23" s="5" t="s">
+        <v>80</v>
+      </c>
       <c r="C23" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="D23" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H23" s="1">
+        <v>8</v>
+      </c>
+      <c r="I23" s="1">
+        <v>0</v>
+      </c>
       <c r="J23" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="3:10" x14ac:dyDescent="0.45">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B24" s="5" t="s">
+        <v>152</v>
+      </c>
       <c r="C24" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="D24" t="s">
+        <v>86</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" t="s">
+        <v>85</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="H24" s="1">
+        <v>2</v>
+      </c>
+      <c r="I24" s="1">
+        <v>57</v>
+      </c>
       <c r="J24" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="3:10" x14ac:dyDescent="0.45">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B25" s="5" t="s">
+        <v>87</v>
+      </c>
       <c r="C25" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="D25" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="H25" s="1">
+        <v>4</v>
+      </c>
+      <c r="I25" s="1">
+        <v>0</v>
+      </c>
       <c r="J25" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="3:10" x14ac:dyDescent="0.45">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="5" t="s">
+        <v>91</v>
+      </c>
       <c r="C26" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="D26" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H26" s="1">
+        <v>2</v>
+      </c>
+      <c r="I26" s="1">
+        <v>0</v>
+      </c>
       <c r="J26" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="3:10" x14ac:dyDescent="0.45">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B27" s="5" t="s">
+        <v>95</v>
+      </c>
       <c r="C27" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="D27" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="H27" s="1">
+        <v>2</v>
+      </c>
+      <c r="I27" s="1">
+        <v>0</v>
+      </c>
       <c r="J27" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="3:10" x14ac:dyDescent="0.45">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B28" s="5" t="s">
+        <v>166</v>
+      </c>
       <c r="C28" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="D28" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="H28" s="1">
+        <v>1</v>
+      </c>
+      <c r="I28" s="1">
+        <v>0</v>
+      </c>
       <c r="J28" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="3:10" x14ac:dyDescent="0.45">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B29" s="5" t="s">
+        <v>99</v>
+      </c>
       <c r="C29" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="D29" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="H29" s="1">
+        <v>1</v>
+      </c>
+      <c r="I29" s="1">
+        <v>0</v>
+      </c>
       <c r="J29" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="3:10" x14ac:dyDescent="0.45">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B30" s="5" t="s">
+        <v>100</v>
+      </c>
       <c r="C30" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="D30" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H30" s="1">
+        <v>1</v>
+      </c>
+      <c r="I30" s="1">
+        <v>0</v>
+      </c>
       <c r="J30" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="3:10" x14ac:dyDescent="0.45">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B31" s="5" t="s">
+        <v>101</v>
+      </c>
       <c r="C31" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="D31" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="H31" s="1">
+        <v>1</v>
+      </c>
+      <c r="I31" s="1">
+        <v>0</v>
+      </c>
       <c r="J31" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="3:10" x14ac:dyDescent="0.45">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B32" s="5" t="s">
+        <v>102</v>
+      </c>
       <c r="C32" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="D32" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="H32" s="1">
+        <v>1</v>
+      </c>
+      <c r="I32" s="1">
+        <v>0</v>
+      </c>
       <c r="J32" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="3:10" x14ac:dyDescent="0.45">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B33" s="5" t="s">
+        <v>103</v>
+      </c>
       <c r="C33" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="D33" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="H33" s="1">
+        <v>2</v>
+      </c>
+      <c r="I33" s="1">
+        <v>0</v>
+      </c>
       <c r="J33" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="3:10" x14ac:dyDescent="0.45">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B34" s="5" t="s">
+        <v>104</v>
+      </c>
       <c r="C34" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="D34" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="H34" s="1">
+        <v>1</v>
+      </c>
+      <c r="I34" s="1">
+        <v>0</v>
+      </c>
       <c r="J34" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="3:10" x14ac:dyDescent="0.45">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B35" s="5" t="s">
+        <v>105</v>
+      </c>
       <c r="C35" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="D35" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="H35" s="1">
+        <v>1</v>
+      </c>
+      <c r="I35" s="1">
+        <v>0</v>
+      </c>
       <c r="J35" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="3:10" x14ac:dyDescent="0.45">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B36" s="5" t="s">
+        <v>106</v>
+      </c>
       <c r="C36" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="D36" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="H36" s="1">
+        <v>1</v>
+      </c>
+      <c r="I36" s="1">
+        <v>0</v>
+      </c>
       <c r="J36" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="3:10" x14ac:dyDescent="0.45">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B37" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="C37" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="D37" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="H37" s="1">
+        <v>1</v>
+      </c>
+      <c r="I37" s="1">
+        <v>0</v>
+      </c>
       <c r="J37" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="3:10" x14ac:dyDescent="0.45">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B38" s="5" t="s">
+        <v>107</v>
+      </c>
       <c r="C38" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="D38" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="H38" s="1">
+        <v>1</v>
+      </c>
+      <c r="I38" s="1">
+        <v>0</v>
+      </c>
       <c r="J38" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="3:10" x14ac:dyDescent="0.45">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B39" s="5" t="s">
+        <v>108</v>
+      </c>
       <c r="C39" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="40" spans="3:10" x14ac:dyDescent="0.45">
+      <c r="D39" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="H39" s="1">
+        <v>1</v>
+      </c>
+      <c r="I39" s="1">
+        <v>0</v>
+      </c>
+      <c r="J39" s="7">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C40" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="41" spans="3:10" x14ac:dyDescent="0.45">
+      <c r="J40" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B41" s="5" t="s">
+        <v>142</v>
+      </c>
       <c r="C41" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="42" spans="3:10" x14ac:dyDescent="0.45">
+      <c r="D41" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="H41" s="1">
+        <v>1</v>
+      </c>
+      <c r="I41" s="1">
+        <v>0</v>
+      </c>
+      <c r="J41" s="7">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B42" s="5" t="s">
+        <v>153</v>
+      </c>
       <c r="C42" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="43" spans="3:10" x14ac:dyDescent="0.45">
+      <c r="D42" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="H42" s="1">
+        <v>1</v>
+      </c>
+      <c r="I42" s="1">
+        <v>0</v>
+      </c>
+      <c r="J42" s="7">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B43" s="5" t="s">
+        <v>159</v>
+      </c>
       <c r="C43" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="44" spans="3:10" x14ac:dyDescent="0.45">
+      <c r="D43" t="s">
+        <v>157</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F43" t="s">
+        <v>158</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="H43" s="1">
+        <v>1</v>
+      </c>
+      <c r="I43" s="1">
+        <v>3</v>
+      </c>
+      <c r="J43" s="7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B44" s="5" t="s">
+        <v>160</v>
+      </c>
       <c r="C44" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="45" spans="3:10" x14ac:dyDescent="0.45">
+      <c r="D44" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="H44" s="1">
+        <v>1</v>
+      </c>
+      <c r="I44" s="1">
+        <v>0</v>
+      </c>
+      <c r="J44" s="7">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C45" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="46" spans="3:10" x14ac:dyDescent="0.45">
+      <c r="J45" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C46" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="47" spans="3:10" x14ac:dyDescent="0.45">
+      <c r="J46" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C47" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="48" spans="3:10" x14ac:dyDescent="0.45">
+      <c r="J47" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C48" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.45">
+      <c r="J48" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C49" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.45">
+      <c r="J49" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C50" s="4" t="s">
         <v>11</v>
+      </c>
+      <c r="J50" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J51" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J52" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J53" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J54" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J55" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J56" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J57" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J58" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J59" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J60" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J61" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J62" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J63" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J64" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J65" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J66" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J67" s="7">
+        <f t="shared" ref="J67:J73" si="1">I67-H67</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J68" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J69" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J70" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J71" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J72" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J73" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1489,8 +2574,40 @@
     <hyperlink ref="B13" r:id="rId6" xr:uid="{A733FADA-82C1-4F90-BED8-B97CB5E0DE63}"/>
     <hyperlink ref="B14" r:id="rId7" xr:uid="{802432F0-11B7-40AA-BF79-E0D5E0CC68B4}"/>
     <hyperlink ref="B15" r:id="rId8" display="https://www.digikey.com/en/products/detail/tdk-corporation/MLF1608E120JT000/613002" xr:uid="{D8A79B70-07C3-44B1-AD38-BD39B6DBBC4F}"/>
+    <hyperlink ref="B16" r:id="rId9" xr:uid="{BBCB6F7F-0749-4637-AC93-49A6061C94F0}"/>
+    <hyperlink ref="B19" r:id="rId10" xr:uid="{FD4DB674-2DB9-4C54-B02D-5CA2F72A7613}"/>
+    <hyperlink ref="B20" r:id="rId11" xr:uid="{D8ECC531-137A-47E3-8E7B-7F5B3E16C0DC}"/>
+    <hyperlink ref="B21" r:id="rId12" xr:uid="{EBF69074-E1AA-4048-89FE-9DC0ACCE9E8B}"/>
+    <hyperlink ref="B22" r:id="rId13" xr:uid="{01721D9B-AAD3-426B-A909-D20253742787}"/>
+    <hyperlink ref="B23" r:id="rId14" xr:uid="{4914439B-4167-460C-853A-EB40DC4CE838}"/>
+    <hyperlink ref="B26" r:id="rId15" xr:uid="{4A2745ED-3370-4564-A62C-B0A1DB78B923}"/>
+    <hyperlink ref="B27" r:id="rId16" xr:uid="{F160F38D-D9AE-42F3-90D2-BC48E8B549E6}"/>
+    <hyperlink ref="B29" r:id="rId17" xr:uid="{EDBFCCEF-AA17-4065-84AE-FA8205AB3657}"/>
+    <hyperlink ref="B30" r:id="rId18" xr:uid="{567E1DFD-7565-4D2B-AD1E-8BA2CC2B7CD1}"/>
+    <hyperlink ref="B31" r:id="rId19" xr:uid="{5724C61A-EE78-499E-8124-DCA88ACE361E}"/>
+    <hyperlink ref="B32" r:id="rId20" xr:uid="{28539F95-762D-44BF-B545-34BCB3608D98}"/>
+    <hyperlink ref="B33" r:id="rId21" xr:uid="{9030104C-9038-4D9B-9262-0388C128CABE}"/>
+    <hyperlink ref="B34" r:id="rId22" xr:uid="{1CBE56DF-2DF3-4E25-83AA-401929945F39}"/>
+    <hyperlink ref="B35" r:id="rId23" xr:uid="{C274C21D-FA45-4B59-8E4E-271C85FFE580}"/>
+    <hyperlink ref="B36" r:id="rId24" xr:uid="{8B0CBE11-CC04-435E-B878-FCBA3CD98D41}"/>
+    <hyperlink ref="B38" r:id="rId25" xr:uid="{AC8432AB-CF64-4FC1-968E-1A353F4F4D5F}"/>
+    <hyperlink ref="B39" r:id="rId26" xr:uid="{C8178E3F-7874-4C86-8929-7A1BB3C402DA}"/>
+    <hyperlink ref="B37" r:id="rId27" xr:uid="{A3E50310-F42D-48EF-81C3-E5BE434F2409}"/>
+    <hyperlink ref="B41" r:id="rId28" xr:uid="{CE69E7BC-8A24-4486-B64F-B95973F21871}"/>
+    <hyperlink ref="B17" r:id="rId29" xr:uid="{D4181B56-5FAB-45CB-89DE-DE8EB259BED5}"/>
+    <hyperlink ref="B2" r:id="rId30" xr:uid="{950B57D0-A0CC-4EBD-B337-7D37E989B726}"/>
+    <hyperlink ref="B4" r:id="rId31" xr:uid="{CD6E5DB5-37E4-4792-AFEC-53589F6D801C}"/>
+    <hyperlink ref="B5" r:id="rId32" xr:uid="{BA151E8C-57CC-464A-877C-C1BC521C019D}"/>
+    <hyperlink ref="B6" r:id="rId33" xr:uid="{547B1D52-F5E0-4AF7-833F-0BFE4EE65081}"/>
+    <hyperlink ref="B10" r:id="rId34" xr:uid="{D906CB7A-FB00-4D76-B1E5-D631D0289074}"/>
+    <hyperlink ref="B24" r:id="rId35" xr:uid="{5DAF8B42-96E1-4E53-BD5E-6450ADB9E014}"/>
+    <hyperlink ref="B42" r:id="rId36" xr:uid="{476A1C4A-31E0-4C93-BE68-9C325C990CE1}"/>
+    <hyperlink ref="B43" r:id="rId37" xr:uid="{D113B403-2FE2-45BB-BAC2-15405AFB41FA}"/>
+    <hyperlink ref="B44" r:id="rId38" xr:uid="{66213E65-08A8-4E8C-81DD-CFF5BE1E8955}"/>
+    <hyperlink ref="B28" r:id="rId39" xr:uid="{726BBFC9-04B4-4769-B4C5-23FB9F7D71A1}"/>
+    <hyperlink ref="B7" r:id="rId40" xr:uid="{CC18A0A0-AA11-4CBF-A10D-1BFFBF4448B2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId9"/>
+  <legacyDrawing r:id="rId41"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Big Acoustics PCB Work
Constructed most circuit blocks in PCB
</commit_message>
<xml_diff>
--- a/TempestBoards/Acoustics/Acoustics BOM.xlsx
+++ b/TempestBoards/Acoustics/Acoustics BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\Documents\Everything\UWRT\Electrical\GIT\electric_boogaloo\TempestBoards\Acoustics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21106A47-94EA-44B7-8673-EF3E525B8C90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D71C9A4-2565-48A4-B93E-C6C36FF75F34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="195">
   <si>
     <t>Distributor</t>
   </si>
@@ -624,6 +624,21 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/w%C3%BCrth-elektronik/885012206089/5453862?s=N4IgTCBcDaIOwGYwFoAcAGddkEZkDkAREAXQF8g</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/ECS-TXO-2520-33-250-AN-TR/XC2258CT-ND/6578565?curr=usd&amp;utm_campaign=buynow&amp;utm_medium=aggregator&amp;utm_source=octopart</t>
+  </si>
+  <si>
+    <t>XC2258TR-ND</t>
+  </si>
+  <si>
+    <t>Crystal</t>
+  </si>
+  <si>
+    <t>ECS-TXO-2520-33-250-AN-TR</t>
+  </si>
+  <si>
+    <t>25 MHz Oscillator</t>
   </si>
 </sst>
 </file>
@@ -828,7 +843,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1128,8 +1143,8 @@
   <dimension ref="B1:M73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I46" sqref="I46"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2509,12 +2524,33 @@
       </c>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B46" s="5" t="s">
+        <v>190</v>
+      </c>
       <c r="C46" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="D46" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="H46" s="1">
+        <v>1</v>
+      </c>
+      <c r="I46" s="1">
+        <v>0</v>
+      </c>
       <c r="J46" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
@@ -2742,8 +2778,9 @@
     <hyperlink ref="B18" r:id="rId42" xr:uid="{67C1310B-8FAC-43CB-9AD5-94640A9C01DE}"/>
     <hyperlink ref="B40" r:id="rId43" xr:uid="{EDEE17FF-68CC-4F30-AB02-AB5170BC04D2}"/>
     <hyperlink ref="B45" r:id="rId44" xr:uid="{039B3AEA-99FA-41CC-A274-C098F368E7D2}"/>
+    <hyperlink ref="B46" r:id="rId45" xr:uid="{29F77E5F-98F8-4F94-8C11-3FA54326F421}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId45"/>
+  <legacyDrawing r:id="rId46"/>
 </worksheet>
 </file>
</xml_diff>